<commit_message>
-Updated the Project Team Information document
</commit_message>
<xml_diff>
--- a/data/CFN KT2017_Project_Team_Information.xlsx
+++ b/data/CFN KT2017_Project_Team_Information.xlsx
@@ -847,7 +847,7 @@
     <t>TVN Project Leader:</t>
   </si>
   <si>
-    <t># weeks individual will participate in Project from June 1, 2015 to May 31, 2016</t>
+    <t># weeks individual will participate in Project from April 1, 2018 to March 31, 2019</t>
   </si>
 </sst>
 </file>
@@ -1507,8 +1507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>

</xml_diff>